<commit_message>
added function to duplicate mode to another mode
</commit_message>
<xml_diff>
--- a/test-tensor-stats.xlsx
+++ b/test-tensor-stats.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meilicharles/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meilicharles/sandbox/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDAF9B18-6908-3249-9685-A12457CADE3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01DC928F-011B-4249-BDEE-1A67474336C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44140" yWindow="7860" windowWidth="16900" windowHeight="12240" xr2:uid="{C05C7466-FC4A-E044-81AA-F9202F062A37}"/>
+    <workbookView xWindow="39180" yWindow="7860" windowWidth="23960" windowHeight="14420" xr2:uid="{C05C7466-FC4A-E044-81AA-F9202F062A37}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>tensor</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t>test3</t>
+  </si>
+  <si>
+    <t>testb1</t>
   </si>
 </sst>
 </file>
@@ -429,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F46AB73D-DB81-DD47-B799-716049E8FF92}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -584,6 +587,11 @@
         <v>32768</v>
       </c>
     </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
trying to add a way to perturb duplicated mode slightly
</commit_message>
<xml_diff>
--- a/test-tensor-stats.xlsx
+++ b/test-tensor-stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meilicharles/sandbox/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01DC928F-011B-4249-BDEE-1A67474336C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3CA376A-6014-6D4A-A586-18FF2E7E19E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39180" yWindow="7860" windowWidth="23960" windowHeight="14420" xr2:uid="{C05C7466-FC4A-E044-81AA-F9202F062A37}"/>
+    <workbookView xWindow="39020" yWindow="7860" windowWidth="23960" windowHeight="14420" xr2:uid="{C05C7466-FC4A-E044-81AA-F9202F062A37}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -435,7 +435,7 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -591,6 +591,36 @@
       <c r="A7" t="s">
         <v>14</v>
       </c>
+      <c r="B7" s="1">
+        <v>0.99519999999999997</v>
+      </c>
+      <c r="C7">
+        <v>210.5</v>
+      </c>
+      <c r="D7">
+        <v>470</v>
+      </c>
+      <c r="E7">
+        <v>77.7</v>
+      </c>
+      <c r="F7">
+        <v>156</v>
+      </c>
+      <c r="G7">
+        <v>1556.5</v>
+      </c>
+      <c r="H7">
+        <v>39810</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0.99</v>
+      </c>
+      <c r="J7">
+        <v>20000</v>
+      </c>
+      <c r="K7">
+        <v>65536</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added correlation matrix script, working on perturbing existing data set
</commit_message>
<xml_diff>
--- a/test-tensor-stats.xlsx
+++ b/test-tensor-stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meilicharles/sandbox/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3CA376A-6014-6D4A-A586-18FF2E7E19E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD61D975-10FD-AF4A-B489-185AF253394B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39020" yWindow="7860" windowWidth="23960" windowHeight="14420" xr2:uid="{C05C7466-FC4A-E044-81AA-F9202F062A37}"/>
+    <workbookView xWindow="12720" yWindow="500" windowWidth="12880" windowHeight="10700" xr2:uid="{C05C7466-FC4A-E044-81AA-F9202F062A37}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>tensor</t>
   </si>
@@ -61,9 +61,6 @@
     <t>median</t>
   </si>
   <si>
-    <t>collisions</t>
-  </si>
-  <si>
     <t>sparsity</t>
   </si>
   <si>
@@ -80,13 +77,29 @@
   </si>
   <si>
     <t>testb1</t>
+  </si>
+  <si>
+    <t>testc3</t>
+  </si>
+  <si>
+    <t>modes</t>
+  </si>
+  <si>
+    <t>testb2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -112,15 +125,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -432,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F46AB73D-DB81-DD47-B799-716049E8FF92}">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -444,7 +461,8 @@
     <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" style="1"/>
+    <col min="8" max="8" width="10.83203125" style="1"/>
+    <col min="9" max="9" width="6.6640625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
@@ -469,17 +487,17 @@
       <c r="G1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>10</v>
-      </c>
-      <c r="K1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -504,13 +522,13 @@
       <c r="G3">
         <v>312.5</v>
       </c>
-      <c r="H3">
-        <v>19936</v>
-      </c>
-      <c r="I3" s="1">
+      <c r="H3" s="1">
         <v>0.99</v>
       </c>
-      <c r="J3">
+      <c r="I3" s="2">
+        <v>3</v>
+      </c>
+      <c r="J3" s="3">
         <v>20000</v>
       </c>
       <c r="K3">
@@ -519,7 +537,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1">
         <v>0.99680000000000002</v>
@@ -539,13 +557,13 @@
       <c r="G4">
         <v>312.5</v>
       </c>
-      <c r="H4">
-        <v>19936</v>
-      </c>
-      <c r="I4" s="1">
+      <c r="H4" s="1">
         <v>0.99</v>
       </c>
-      <c r="J4">
+      <c r="I4" s="2">
+        <v>3</v>
+      </c>
+      <c r="J4" s="3">
         <v>20000</v>
       </c>
       <c r="K4">
@@ -554,7 +572,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1">
         <v>0.99680000000000002</v>
@@ -574,13 +592,13 @@
       <c r="G5">
         <v>312.5</v>
       </c>
-      <c r="H5">
-        <v>19936</v>
-      </c>
-      <c r="I5" s="1">
+      <c r="H5" s="1">
         <v>0.99</v>
       </c>
-      <c r="J5">
+      <c r="I5" s="2">
+        <v>3</v>
+      </c>
+      <c r="J5" s="3">
         <v>20000</v>
       </c>
       <c r="K5">
@@ -589,7 +607,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" s="1">
         <v>0.99519999999999997</v>
@@ -609,17 +627,81 @@
       <c r="G7">
         <v>1556.5</v>
       </c>
-      <c r="H7">
-        <v>39810</v>
-      </c>
-      <c r="I7" s="1">
+      <c r="H7" s="1">
         <v>0.99</v>
       </c>
-      <c r="J7">
+      <c r="I7" s="2">
+        <v>3</v>
+      </c>
+      <c r="J7" s="3">
         <v>20000</v>
       </c>
       <c r="K7">
         <v>65536</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0.99850000000000005</v>
+      </c>
+      <c r="C8">
+        <v>651.79999999999995</v>
+      </c>
+      <c r="D8">
+        <v>1466</v>
+      </c>
+      <c r="E8">
+        <v>231.8</v>
+      </c>
+      <c r="F8">
+        <v>488</v>
+      </c>
+      <c r="G8">
+        <v>489</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0.99</v>
+      </c>
+      <c r="I8" s="2">
+        <v>3</v>
+      </c>
+      <c r="J8" s="3">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0.99809999999999999</v>
+      </c>
+      <c r="C13">
+        <v>523.5</v>
+      </c>
+      <c r="D13">
+        <v>1173</v>
+      </c>
+      <c r="E13">
+        <v>189.3</v>
+      </c>
+      <c r="F13">
+        <v>391</v>
+      </c>
+      <c r="G13">
+        <v>391</v>
+      </c>
+      <c r="H13" s="1">
+        <v>0.99</v>
+      </c>
+      <c r="I13" s="2">
+        <v>4</v>
+      </c>
+      <c r="J13" s="3">
+        <v>50000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>